<commit_message>
adding images and updating protocol
</commit_message>
<xml_diff>
--- a/newMetadata/metadata_17Apr2023.xlsx
+++ b/newMetadata/metadata_17Apr2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mab/Documents/GitHub/bryozoa/stegino_metadata/newMetadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1D11EA-EFCC-D44A-970A-E76FD7FB257A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BFF8DD-6E90-B14E-BFA9-D273036C47BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="820" windowWidth="26040" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16328" uniqueCount="3125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17225" uniqueCount="3349">
   <si>
     <t>formation</t>
   </si>
@@ -9409,6 +9409,678 @@
   </si>
   <si>
     <t>locality code</t>
+  </si>
+  <si>
+    <t>Modern</t>
+  </si>
+  <si>
+    <t>MAB</t>
+  </si>
+  <si>
+    <t>NL-23</t>
+  </si>
+  <si>
+    <t>previousSpecimenID</t>
+  </si>
+  <si>
+    <t>NL23 #1</t>
+  </si>
+  <si>
+    <t>1200_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1200_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01201_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01201_CC</t>
+  </si>
+  <si>
+    <t>10/30/2023</t>
+  </si>
+  <si>
+    <t>1201_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS-2</t>
+  </si>
+  <si>
+    <t>TS2 #2</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>only photographed largest piece</t>
+  </si>
+  <si>
+    <t>01201_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1201_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01202_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01202_CC</t>
+  </si>
+  <si>
+    <t>1202_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS-12</t>
+  </si>
+  <si>
+    <t>TS12 #8</t>
+  </si>
+  <si>
+    <t>01202_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1202_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01203_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01203_CC</t>
+  </si>
+  <si>
+    <t>1203_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>NL23 #3</t>
+  </si>
+  <si>
+    <t>are these magnifica?</t>
+  </si>
+  <si>
+    <t>01203_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01203_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1203_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1203_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01204_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01204_CC</t>
+  </si>
+  <si>
+    <t>1204_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS12 #5</t>
+  </si>
+  <si>
+    <t>01204_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1204_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01204_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1204_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01205_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1205_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>NL23 #5</t>
+  </si>
+  <si>
+    <t>01205_CC</t>
+  </si>
+  <si>
+    <t>01205_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1205_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01205_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1205_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01205_CC_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1205_CC_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01206_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01206_CC</t>
+  </si>
+  <si>
+    <t>1206_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS2 #5</t>
+  </si>
+  <si>
+    <t>specimen A</t>
+  </si>
+  <si>
+    <t>01206_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01206_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>specimen B</t>
+  </si>
+  <si>
+    <t>01207_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01207_CC</t>
+  </si>
+  <si>
+    <t>1207_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1206_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1206_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS12 #6</t>
+  </si>
+  <si>
+    <t>01207_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1207_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01207_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1207_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01207_CC_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1207_CC_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01207_CC_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1207_CC_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01207_CV_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01207_CV</t>
+  </si>
+  <si>
+    <t>1207_CV_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1207CC is the same shell but different colony as 1207CV</t>
+  </si>
+  <si>
+    <t>1207CV is the same shell but different colony as 1207CC</t>
+  </si>
+  <si>
+    <t>01207_CV_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1207_CV_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01207_CV_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1207_CV_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01207_CV_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1207_CV_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01207_CV_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1207_CV_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01208_CV_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01208_CV</t>
+  </si>
+  <si>
+    <t>1208_CV_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>NL-01</t>
+  </si>
+  <si>
+    <t>NL01 #1</t>
+  </si>
+  <si>
+    <t>largest piece</t>
+  </si>
+  <si>
+    <t>01208_CV_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01208_CV_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01208_CV_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1208_CV_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1208_CV_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1208_CV_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01209_CC</t>
+  </si>
+  <si>
+    <t>1209_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>Could not get image of CV side</t>
+  </si>
+  <si>
+    <t>01209_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01209_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01209_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01209_CC_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01209_CC_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1209_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1209_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1209_CC_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1209_CC_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01210_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01210_CC</t>
+  </si>
+  <si>
+    <t>1210_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS12 #4</t>
+  </si>
+  <si>
+    <t>01211_CV_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01211_CV</t>
+  </si>
+  <si>
+    <t>1211_CV_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS12 #3</t>
+  </si>
+  <si>
+    <t>01211_CV_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1211_CV_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01211_CV_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1211_CV_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01212_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01212_CC</t>
+  </si>
+  <si>
+    <t>1212_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS12 #1</t>
+  </si>
+  <si>
+    <t>01212_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1212_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01213_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01213_CC</t>
+  </si>
+  <si>
+    <t>1213_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS-3</t>
+  </si>
+  <si>
+    <t>TS3 #1</t>
+  </si>
+  <si>
+    <t>01213_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1213_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01214_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01214_CC</t>
+  </si>
+  <si>
+    <t>1214_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS2 #4</t>
+  </si>
+  <si>
+    <t>01214_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1214_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01215_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01215_CC</t>
+  </si>
+  <si>
+    <t>1215_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS2 #1</t>
+  </si>
+  <si>
+    <t>01215_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1215_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01216_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01216_CC</t>
+  </si>
+  <si>
+    <t>1216_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>NL23 #2</t>
+  </si>
+  <si>
+    <t>01216_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1216_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01216_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1216_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01217_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01217_CC</t>
+  </si>
+  <si>
+    <t>11/13/2023</t>
+  </si>
+  <si>
+    <t>1217_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>NL01 #2</t>
+  </si>
+  <si>
+    <t>1217CV is the same shell but different colony as 1217CC</t>
+  </si>
+  <si>
+    <t>01217_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1217_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01217_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1217_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01217_CC_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1217_CC_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01217_CC_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1217_CC_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01217_CC_6_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1217_CC_6_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01217_CV_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01217_CV</t>
+  </si>
+  <si>
+    <t>1217_CV_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1217CC is the same shell but different colony as 1217CV</t>
+  </si>
+  <si>
+    <t>01217_CV_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1217_CV_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01217_CV_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1217_CV_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01217_CV_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1217_CV_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01218_CV_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01218_CV</t>
+  </si>
+  <si>
+    <t>1218_CV_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS12 #7</t>
+  </si>
+  <si>
+    <t>01218_CV_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1218_CV_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01218_CV_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1218_CV_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01218_CV_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1218_CV_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01218_CV_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1218_CV_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01219_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01219_CC</t>
+  </si>
+  <si>
+    <t>1219_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS2 #3</t>
+  </si>
+  <si>
+    <t>01219_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1219_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01220_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01220_CC</t>
+  </si>
+  <si>
+    <t>1220_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>NL23 #4</t>
+  </si>
+  <si>
+    <t>01220_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1220_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>all four pieces; first two are largest piece; magnifica?</t>
+  </si>
+  <si>
+    <t>all four pieces; second largest piece; magnifica?</t>
+  </si>
+  <si>
+    <t>1220_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01220_CC_3_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01220_CC_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1220_CC_4_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01220_CC_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1220_CC_5_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>all four pieces; third largest piece; magnifica?</t>
+  </si>
+  <si>
+    <t>01220_CC_6_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1220_CC_6_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>all four pieces; fourth (smallest) largest piece; magnifica?</t>
+  </si>
+  <si>
+    <t>01221_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>01221_CC</t>
+  </si>
+  <si>
+    <t>1221_CC_1_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>TS12 #2</t>
+  </si>
+  <si>
+    <t>largest piece; originally says TS2, but already have a TS2 and am missing a TS12 and suspect it was an error (see note)</t>
+  </si>
+  <si>
+    <t>01221_CC_2_15v_x30_BSE</t>
+  </si>
+  <si>
+    <t>1221_CC_2_15v_x30_BSE</t>
   </si>
 </sst>
 </file>
@@ -10258,11 +10930,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1891"/>
+  <dimension ref="A1:Q1969"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1858" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1892" sqref="A1892"/>
+      <pane ySplit="1" topLeftCell="A1940" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1970" sqref="A1970"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10272,7 +10944,7 @@
     <col min="5" max="10" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>318</v>
       </c>
@@ -10318,8 +10990,14 @@
       <c r="O1" t="s">
         <v>3124</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>3128</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>3138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>334</v>
       </c>
@@ -10351,7 +11029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>334</v>
       </c>
@@ -10383,7 +11061,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>335</v>
       </c>
@@ -10415,7 +11093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>335</v>
       </c>
@@ -10447,7 +11125,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>336</v>
       </c>
@@ -10479,7 +11157,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>337</v>
       </c>
@@ -10511,7 +11189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>338</v>
       </c>
@@ -10543,7 +11221,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>339</v>
       </c>
@@ -10575,7 +11253,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>340</v>
       </c>
@@ -10607,7 +11285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>341</v>
       </c>
@@ -10639,7 +11317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>342</v>
       </c>
@@ -10671,7 +11349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>342</v>
       </c>
@@ -10703,7 +11381,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>343</v>
       </c>
@@ -10735,7 +11413,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>344</v>
       </c>
@@ -10767,7 +11445,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>345</v>
       </c>
@@ -70708,7 +71386,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1889" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1889" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1889" t="s">
         <v>2213</v>
       </c>
@@ -70740,7 +71418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1890" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1890" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1890" t="s">
         <v>2214</v>
       </c>
@@ -70772,7 +71450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1891" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1891" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1891" t="s">
         <v>2215</v>
       </c>
@@ -70802,6 +71480,3141 @@
       </c>
       <c r="J1891" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="1892" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1892" t="s">
+        <v>2040</v>
+      </c>
+      <c r="B1892" t="s">
+        <v>2347</v>
+      </c>
+      <c r="C1892" s="1">
+        <v>45270</v>
+      </c>
+      <c r="D1892" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1892" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1892">
+        <v>30</v>
+      </c>
+      <c r="G1892" t="s">
+        <v>3130</v>
+      </c>
+      <c r="H1892" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1892" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1892" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1892" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1892" t="s">
+        <v>3129</v>
+      </c>
+    </row>
+    <row r="1893" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1893" t="s">
+        <v>2041</v>
+      </c>
+      <c r="B1893" t="s">
+        <v>2347</v>
+      </c>
+      <c r="C1893" s="1">
+        <v>45270</v>
+      </c>
+      <c r="D1893" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1893" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1893">
+        <v>30</v>
+      </c>
+      <c r="G1893" t="s">
+        <v>3131</v>
+      </c>
+      <c r="H1893" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1893" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1893" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1893" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1893" t="s">
+        <v>3129</v>
+      </c>
+    </row>
+    <row r="1894" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1894" t="s">
+        <v>3132</v>
+      </c>
+      <c r="B1894" t="s">
+        <v>3133</v>
+      </c>
+      <c r="C1894" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1894" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1894" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1894">
+        <v>30</v>
+      </c>
+      <c r="G1894" t="s">
+        <v>3135</v>
+      </c>
+      <c r="H1894" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1894" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1894" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1894" t="s">
+        <v>3136</v>
+      </c>
+      <c r="P1894" t="s">
+        <v>3137</v>
+      </c>
+      <c r="Q1894" t="s">
+        <v>3139</v>
+      </c>
+    </row>
+    <row r="1895" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1895" t="s">
+        <v>3140</v>
+      </c>
+      <c r="B1895" t="s">
+        <v>3133</v>
+      </c>
+      <c r="C1895" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1895" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1895" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1895">
+        <v>30</v>
+      </c>
+      <c r="G1895" t="s">
+        <v>3141</v>
+      </c>
+      <c r="H1895" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1895" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1895" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1895" t="s">
+        <v>3136</v>
+      </c>
+      <c r="P1895" t="s">
+        <v>3137</v>
+      </c>
+      <c r="Q1895" t="s">
+        <v>3139</v>
+      </c>
+    </row>
+    <row r="1896" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1896" t="s">
+        <v>3142</v>
+      </c>
+      <c r="B1896" t="s">
+        <v>3143</v>
+      </c>
+      <c r="C1896" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1896" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1896" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1896">
+        <v>30</v>
+      </c>
+      <c r="G1896" t="s">
+        <v>3144</v>
+      </c>
+      <c r="H1896" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1896" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1896" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1896" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1896" t="s">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="1897" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1897" t="s">
+        <v>3147</v>
+      </c>
+      <c r="B1897" t="s">
+        <v>3143</v>
+      </c>
+      <c r="C1897" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1897" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1897" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1897">
+        <v>30</v>
+      </c>
+      <c r="G1897" t="s">
+        <v>3148</v>
+      </c>
+      <c r="H1897" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1897" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1897" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1897" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1897" t="s">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="1898" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1898" t="s">
+        <v>3149</v>
+      </c>
+      <c r="B1898" t="s">
+        <v>3150</v>
+      </c>
+      <c r="C1898" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1898" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1898" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1898">
+        <v>30</v>
+      </c>
+      <c r="G1898" t="s">
+        <v>3151</v>
+      </c>
+      <c r="H1898" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1898" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1898" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1898" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1898" t="s">
+        <v>3152</v>
+      </c>
+      <c r="Q1898" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="1899" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1899" t="s">
+        <v>3154</v>
+      </c>
+      <c r="B1899" t="s">
+        <v>3150</v>
+      </c>
+      <c r="C1899" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1899" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1899" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1899">
+        <v>30</v>
+      </c>
+      <c r="G1899" t="s">
+        <v>3157</v>
+      </c>
+      <c r="H1899" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1899" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1899" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1899" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1899" t="s">
+        <v>3152</v>
+      </c>
+      <c r="Q1899" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="1900" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1900" t="s">
+        <v>3155</v>
+      </c>
+      <c r="B1900" t="s">
+        <v>3150</v>
+      </c>
+      <c r="C1900" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1900" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1900" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1900">
+        <v>30</v>
+      </c>
+      <c r="G1900" t="s">
+        <v>3156</v>
+      </c>
+      <c r="H1900" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1900" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1900" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1900" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1900" t="s">
+        <v>3152</v>
+      </c>
+      <c r="Q1900" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="1901" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1901" t="s">
+        <v>3158</v>
+      </c>
+      <c r="B1901" t="s">
+        <v>3159</v>
+      </c>
+      <c r="C1901" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1901" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1901" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1901">
+        <v>30</v>
+      </c>
+      <c r="G1901" t="s">
+        <v>3160</v>
+      </c>
+      <c r="H1901" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1901" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1901" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1901" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1901" t="s">
+        <v>3161</v>
+      </c>
+    </row>
+    <row r="1902" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1902" t="s">
+        <v>3162</v>
+      </c>
+      <c r="B1902" t="s">
+        <v>3159</v>
+      </c>
+      <c r="C1902" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1902" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1902" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1902">
+        <v>30</v>
+      </c>
+      <c r="G1902" t="s">
+        <v>3163</v>
+      </c>
+      <c r="H1902" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1902" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1902" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1902" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1902" t="s">
+        <v>3161</v>
+      </c>
+    </row>
+    <row r="1903" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1903" t="s">
+        <v>3164</v>
+      </c>
+      <c r="B1903" t="s">
+        <v>3159</v>
+      </c>
+      <c r="C1903" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1903" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1903" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1903">
+        <v>30</v>
+      </c>
+      <c r="G1903" t="s">
+        <v>3165</v>
+      </c>
+      <c r="H1903" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1903" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1903" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1903" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1903" t="s">
+        <v>3161</v>
+      </c>
+    </row>
+    <row r="1904" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1904" t="s">
+        <v>3166</v>
+      </c>
+      <c r="B1904" t="s">
+        <v>3169</v>
+      </c>
+      <c r="C1904" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1904" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1904" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1904">
+        <v>30</v>
+      </c>
+      <c r="G1904" t="s">
+        <v>3167</v>
+      </c>
+      <c r="H1904" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1904" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1904" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1904" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1904" t="s">
+        <v>3168</v>
+      </c>
+      <c r="Q1904" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="1905" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1905" t="s">
+        <v>3170</v>
+      </c>
+      <c r="B1905" t="s">
+        <v>3169</v>
+      </c>
+      <c r="C1905" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1905" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1905" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1905">
+        <v>30</v>
+      </c>
+      <c r="G1905" t="s">
+        <v>3171</v>
+      </c>
+      <c r="H1905" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1905" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1905" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1905" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1905" t="s">
+        <v>3168</v>
+      </c>
+      <c r="Q1905" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="1906" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1906" t="s">
+        <v>3172</v>
+      </c>
+      <c r="B1906" t="s">
+        <v>3169</v>
+      </c>
+      <c r="C1906" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1906" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1906" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1906">
+        <v>30</v>
+      </c>
+      <c r="G1906" t="s">
+        <v>3173</v>
+      </c>
+      <c r="H1906" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1906" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1906" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1906" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1906" t="s">
+        <v>3168</v>
+      </c>
+      <c r="Q1906" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="1907" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1907" t="s">
+        <v>3174</v>
+      </c>
+      <c r="B1907" t="s">
+        <v>3169</v>
+      </c>
+      <c r="C1907" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1907" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1907" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1907">
+        <v>30</v>
+      </c>
+      <c r="G1907" t="s">
+        <v>3175</v>
+      </c>
+      <c r="H1907" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1907" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1907" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1907" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1907" t="s">
+        <v>3168</v>
+      </c>
+      <c r="Q1907" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="1908" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1908" t="s">
+        <v>3176</v>
+      </c>
+      <c r="B1908" t="s">
+        <v>3177</v>
+      </c>
+      <c r="C1908" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1908" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1908" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1908">
+        <v>30</v>
+      </c>
+      <c r="G1908" t="s">
+        <v>3178</v>
+      </c>
+      <c r="H1908" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1908" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1908" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1908" t="s">
+        <v>3136</v>
+      </c>
+      <c r="P1908" t="s">
+        <v>3179</v>
+      </c>
+      <c r="Q1908" t="s">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="1909" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1909" t="s">
+        <v>3181</v>
+      </c>
+      <c r="B1909" t="s">
+        <v>3177</v>
+      </c>
+      <c r="C1909" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1909" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1909" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1909">
+        <v>30</v>
+      </c>
+      <c r="G1909" t="s">
+        <v>3187</v>
+      </c>
+      <c r="H1909" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1909" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1909" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1909" t="s">
+        <v>3136</v>
+      </c>
+      <c r="P1909" t="s">
+        <v>3179</v>
+      </c>
+      <c r="Q1909" t="s">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="1910" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1910" t="s">
+        <v>3182</v>
+      </c>
+      <c r="B1910" t="s">
+        <v>3177</v>
+      </c>
+      <c r="C1910" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1910" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1910" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1910">
+        <v>30</v>
+      </c>
+      <c r="G1910" t="s">
+        <v>3188</v>
+      </c>
+      <c r="H1910" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1910" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1910" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1910" t="s">
+        <v>3136</v>
+      </c>
+      <c r="P1910" t="s">
+        <v>3179</v>
+      </c>
+      <c r="Q1910" t="s">
+        <v>3183</v>
+      </c>
+    </row>
+    <row r="1911" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1911" t="s">
+        <v>3184</v>
+      </c>
+      <c r="B1911" t="s">
+        <v>3185</v>
+      </c>
+      <c r="C1911" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1911" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1911" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1911">
+        <v>30</v>
+      </c>
+      <c r="G1911" t="s">
+        <v>3186</v>
+      </c>
+      <c r="H1911" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1911" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1911" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1911" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1911" t="s">
+        <v>3189</v>
+      </c>
+      <c r="Q1911" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="1912" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1912" t="s">
+        <v>3190</v>
+      </c>
+      <c r="B1912" t="s">
+        <v>3185</v>
+      </c>
+      <c r="C1912" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1912" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1912" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1912">
+        <v>30</v>
+      </c>
+      <c r="G1912" t="s">
+        <v>3191</v>
+      </c>
+      <c r="H1912" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1912" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1912" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1912" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1912" t="s">
+        <v>3189</v>
+      </c>
+      <c r="Q1912" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="1913" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1913" t="s">
+        <v>3192</v>
+      </c>
+      <c r="B1913" t="s">
+        <v>3185</v>
+      </c>
+      <c r="C1913" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1913" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1913" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1913">
+        <v>30</v>
+      </c>
+      <c r="G1913" t="s">
+        <v>3193</v>
+      </c>
+      <c r="H1913" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1913" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1913" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1913" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1913" t="s">
+        <v>3189</v>
+      </c>
+      <c r="Q1913" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="1914" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1914" t="s">
+        <v>3194</v>
+      </c>
+      <c r="B1914" t="s">
+        <v>3185</v>
+      </c>
+      <c r="C1914" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1914" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1914" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1914">
+        <v>30</v>
+      </c>
+      <c r="G1914" t="s">
+        <v>3195</v>
+      </c>
+      <c r="H1914" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1914" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1914" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1914" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1914" t="s">
+        <v>3189</v>
+      </c>
+      <c r="Q1914" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="1915" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1915" t="s">
+        <v>3196</v>
+      </c>
+      <c r="B1915" t="s">
+        <v>3185</v>
+      </c>
+      <c r="C1915" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1915" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1915" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1915">
+        <v>30</v>
+      </c>
+      <c r="G1915" t="s">
+        <v>3197</v>
+      </c>
+      <c r="H1915" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1915" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1915" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1915" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1915" t="s">
+        <v>3189</v>
+      </c>
+      <c r="Q1915" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="1916" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1916" t="s">
+        <v>3198</v>
+      </c>
+      <c r="B1916" t="s">
+        <v>3199</v>
+      </c>
+      <c r="C1916" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1916" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1916" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1916">
+        <v>30</v>
+      </c>
+      <c r="G1916" t="s">
+        <v>3200</v>
+      </c>
+      <c r="H1916" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1916" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1916" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1916" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1916" t="s">
+        <v>3189</v>
+      </c>
+      <c r="Q1916" t="s">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="1917" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1917" t="s">
+        <v>3203</v>
+      </c>
+      <c r="B1917" t="s">
+        <v>3199</v>
+      </c>
+      <c r="C1917" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1917" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1917" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1917">
+        <v>30</v>
+      </c>
+      <c r="G1917" t="s">
+        <v>3204</v>
+      </c>
+      <c r="H1917" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1917" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1917" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1917" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1917" t="s">
+        <v>3189</v>
+      </c>
+      <c r="Q1917" t="s">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="1918" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1918" s="2" t="s">
+        <v>3205</v>
+      </c>
+      <c r="B1918" s="2" t="s">
+        <v>3199</v>
+      </c>
+      <c r="C1918" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1918" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1918" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1918" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1918" s="2" t="s">
+        <v>3206</v>
+      </c>
+      <c r="H1918" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1918" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1918" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="K1918" s="2"/>
+      <c r="L1918" s="2"/>
+      <c r="M1918" s="2"/>
+      <c r="N1918" s="2"/>
+      <c r="O1918" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1918" s="2" t="s">
+        <v>3189</v>
+      </c>
+      <c r="Q1918" s="2" t="s">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="1919" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1919" s="2" t="s">
+        <v>3207</v>
+      </c>
+      <c r="B1919" s="2" t="s">
+        <v>3199</v>
+      </c>
+      <c r="C1919" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1919" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1919" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1919" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1919" s="2" t="s">
+        <v>3208</v>
+      </c>
+      <c r="H1919" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1919" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1919" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="K1919" s="2"/>
+      <c r="L1919" s="2"/>
+      <c r="M1919" s="2"/>
+      <c r="N1919" s="2"/>
+      <c r="O1919" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1919" s="2" t="s">
+        <v>3189</v>
+      </c>
+      <c r="Q1919" s="2" t="s">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="1920" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1920" s="2" t="s">
+        <v>3209</v>
+      </c>
+      <c r="B1920" s="2" t="s">
+        <v>3199</v>
+      </c>
+      <c r="C1920" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1920" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1920" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1920" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1920" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="H1920" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1920" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1920" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="K1920" s="2"/>
+      <c r="L1920" s="2"/>
+      <c r="M1920" s="2"/>
+      <c r="N1920" s="2"/>
+      <c r="O1920" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1920" s="2" t="s">
+        <v>3189</v>
+      </c>
+      <c r="Q1920" s="2" t="s">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="1921" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1921" s="2" t="s">
+        <v>3211</v>
+      </c>
+      <c r="B1921" s="2" t="s">
+        <v>3212</v>
+      </c>
+      <c r="C1921" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1921" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1921" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1921" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1921" s="2" t="s">
+        <v>3213</v>
+      </c>
+      <c r="H1921" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1921" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1921" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1921" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1921" s="2" t="s">
+        <v>3215</v>
+      </c>
+      <c r="Q1921" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="1922" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1922" s="2" t="s">
+        <v>3217</v>
+      </c>
+      <c r="B1922" s="2" t="s">
+        <v>3212</v>
+      </c>
+      <c r="C1922" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1922" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1922" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1922" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1922" s="2" t="s">
+        <v>3220</v>
+      </c>
+      <c r="H1922" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1922" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1922" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1922" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1922" s="2" t="s">
+        <v>3215</v>
+      </c>
+      <c r="Q1922" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="1923" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1923" s="2" t="s">
+        <v>3218</v>
+      </c>
+      <c r="B1923" s="2" t="s">
+        <v>3212</v>
+      </c>
+      <c r="C1923" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1923" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1923" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1923" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1923" s="2" t="s">
+        <v>3221</v>
+      </c>
+      <c r="H1923" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1923" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1923" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1923" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1923" s="2" t="s">
+        <v>3215</v>
+      </c>
+      <c r="Q1923" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="1924" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1924" s="2" t="s">
+        <v>3219</v>
+      </c>
+      <c r="B1924" s="2" t="s">
+        <v>3212</v>
+      </c>
+      <c r="C1924" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1924" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1924" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1924" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1924" s="2" t="s">
+        <v>3222</v>
+      </c>
+      <c r="H1924" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1924" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1924" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1924" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1924" s="2" t="s">
+        <v>3215</v>
+      </c>
+      <c r="Q1924" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="1925" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1925" s="2" t="s">
+        <v>3226</v>
+      </c>
+      <c r="B1925" s="2" t="s">
+        <v>3223</v>
+      </c>
+      <c r="C1925" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1925" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1925" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1925" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1925" s="2" t="s">
+        <v>3224</v>
+      </c>
+      <c r="H1925" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1925" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1925" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1925" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1925" s="2" t="s">
+        <v>3215</v>
+      </c>
+      <c r="Q1925" t="s">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="1926" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1926" s="2" t="s">
+        <v>3227</v>
+      </c>
+      <c r="B1926" s="2" t="s">
+        <v>3223</v>
+      </c>
+      <c r="C1926" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1926" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1926" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1926" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1926" s="2" t="s">
+        <v>3231</v>
+      </c>
+      <c r="H1926" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1926" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1926" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1926" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1926" s="2" t="s">
+        <v>3215</v>
+      </c>
+      <c r="Q1926" t="s">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="1927" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1927" s="2" t="s">
+        <v>3228</v>
+      </c>
+      <c r="B1927" s="2" t="s">
+        <v>3223</v>
+      </c>
+      <c r="C1927" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1927" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1927" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1927" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1927" s="2" t="s">
+        <v>3232</v>
+      </c>
+      <c r="H1927" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1927" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1927" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1927" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1927" s="2" t="s">
+        <v>3215</v>
+      </c>
+      <c r="Q1927" t="s">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="1928" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1928" s="2" t="s">
+        <v>3229</v>
+      </c>
+      <c r="B1928" s="2" t="s">
+        <v>3223</v>
+      </c>
+      <c r="C1928" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1928" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1928" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1928" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1928" s="2" t="s">
+        <v>3233</v>
+      </c>
+      <c r="H1928" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1928" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1928" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1928" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1928" s="2" t="s">
+        <v>3215</v>
+      </c>
+      <c r="Q1928" t="s">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="1929" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1929" s="2" t="s">
+        <v>3230</v>
+      </c>
+      <c r="B1929" s="2" t="s">
+        <v>3223</v>
+      </c>
+      <c r="C1929" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1929" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1929" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1929" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1929" s="2" t="s">
+        <v>3234</v>
+      </c>
+      <c r="H1929" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1929" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1929" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1929" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1929" s="2" t="s">
+        <v>3215</v>
+      </c>
+      <c r="Q1929" t="s">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="1930" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1930" s="2" t="s">
+        <v>3235</v>
+      </c>
+      <c r="B1930" s="2" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C1930" s="2" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1930" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1930" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1930" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1930" s="2" t="s">
+        <v>3237</v>
+      </c>
+      <c r="H1930" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1930" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1930" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1930" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1930" s="2" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="1931" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1931" s="2" t="s">
+        <v>3239</v>
+      </c>
+      <c r="B1931" s="2" t="s">
+        <v>3240</v>
+      </c>
+      <c r="C1931" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1931" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1931" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1931" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1931" s="2" t="s">
+        <v>3241</v>
+      </c>
+      <c r="H1931" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1931" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1931" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1931" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1931" s="2" t="s">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="1932" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1932" s="2" t="s">
+        <v>3243</v>
+      </c>
+      <c r="B1932" s="2" t="s">
+        <v>3240</v>
+      </c>
+      <c r="C1932" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1932" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1932" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1932" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1932" s="2" t="s">
+        <v>3244</v>
+      </c>
+      <c r="H1932" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1932" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1932" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1932" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1932" s="2" t="s">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="1933" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1933" s="2" t="s">
+        <v>3245</v>
+      </c>
+      <c r="B1933" s="2" t="s">
+        <v>3240</v>
+      </c>
+      <c r="C1933" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1933" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1933" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1933" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1933" s="2" t="s">
+        <v>3246</v>
+      </c>
+      <c r="H1933" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1933" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1933" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1933" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1933" s="2" t="s">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="1934" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1934" s="2" t="s">
+        <v>3247</v>
+      </c>
+      <c r="B1934" s="2" t="s">
+        <v>3248</v>
+      </c>
+      <c r="C1934" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1934" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1934" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1934" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1934" s="2" t="s">
+        <v>3249</v>
+      </c>
+      <c r="H1934" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1934" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1934" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1934" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1934" s="2" t="s">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="1935" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1935" s="2" t="s">
+        <v>3251</v>
+      </c>
+      <c r="B1935" s="2" t="s">
+        <v>3248</v>
+      </c>
+      <c r="C1935" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1935" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1935" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1935" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1935" s="2" t="s">
+        <v>3252</v>
+      </c>
+      <c r="H1935" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1935" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1935" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1935" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1935" s="2" t="s">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="1936" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1936" s="2" t="s">
+        <v>3253</v>
+      </c>
+      <c r="B1936" s="2" t="s">
+        <v>3254</v>
+      </c>
+      <c r="C1936" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1936" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1936" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1936" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1936" s="2" t="s">
+        <v>3255</v>
+      </c>
+      <c r="H1936" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1936" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1936" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1936" s="2" t="s">
+        <v>3256</v>
+      </c>
+      <c r="P1936" s="2" t="s">
+        <v>3257</v>
+      </c>
+    </row>
+    <row r="1937" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1937" s="2" t="s">
+        <v>3258</v>
+      </c>
+      <c r="B1937" s="2" t="s">
+        <v>3254</v>
+      </c>
+      <c r="C1937" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1937" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1937" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1937" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1937" s="2" t="s">
+        <v>3259</v>
+      </c>
+      <c r="H1937" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1937" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1937" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1937" s="2" t="s">
+        <v>3256</v>
+      </c>
+      <c r="P1937" s="2" t="s">
+        <v>3257</v>
+      </c>
+    </row>
+    <row r="1938" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1938" s="2" t="s">
+        <v>3260</v>
+      </c>
+      <c r="B1938" s="2" t="s">
+        <v>3261</v>
+      </c>
+      <c r="C1938" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1938" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1938" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1938" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1938" s="2" t="s">
+        <v>3262</v>
+      </c>
+      <c r="H1938" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1938" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1938" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1938" s="2" t="s">
+        <v>3136</v>
+      </c>
+      <c r="P1938" s="2" t="s">
+        <v>3263</v>
+      </c>
+    </row>
+    <row r="1939" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1939" s="2" t="s">
+        <v>3264</v>
+      </c>
+      <c r="B1939" s="2" t="s">
+        <v>3261</v>
+      </c>
+      <c r="C1939" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1939" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1939" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1939" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1939" s="2" t="s">
+        <v>3265</v>
+      </c>
+      <c r="H1939" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1939" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1939" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1939" s="2" t="s">
+        <v>3136</v>
+      </c>
+      <c r="P1939" s="2" t="s">
+        <v>3263</v>
+      </c>
+    </row>
+    <row r="1940" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1940" s="2" t="s">
+        <v>3266</v>
+      </c>
+      <c r="B1940" s="2" t="s">
+        <v>3267</v>
+      </c>
+      <c r="C1940" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1940" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1940" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1940" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1940" s="2" t="s">
+        <v>3268</v>
+      </c>
+      <c r="H1940" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1940" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1940" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1940" s="2" t="s">
+        <v>3136</v>
+      </c>
+      <c r="P1940" s="2" t="s">
+        <v>3269</v>
+      </c>
+      <c r="Q1940" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="1941" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1941" s="2" t="s">
+        <v>3270</v>
+      </c>
+      <c r="B1941" s="2" t="s">
+        <v>3267</v>
+      </c>
+      <c r="C1941" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1941" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1941" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1941" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1941" s="2" t="s">
+        <v>3271</v>
+      </c>
+      <c r="H1941" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1941" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1941" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1941" s="2" t="s">
+        <v>3136</v>
+      </c>
+      <c r="P1941" s="2" t="s">
+        <v>3269</v>
+      </c>
+      <c r="Q1941" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="1942" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1942" s="2" t="s">
+        <v>3272</v>
+      </c>
+      <c r="B1942" s="2" t="s">
+        <v>3273</v>
+      </c>
+      <c r="C1942" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1942" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1942" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1942" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1942" s="2" t="s">
+        <v>3274</v>
+      </c>
+      <c r="H1942" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1942" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1942" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1942" s="2" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1942" s="2" t="s">
+        <v>3275</v>
+      </c>
+    </row>
+    <row r="1943" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1943" s="2" t="s">
+        <v>3276</v>
+      </c>
+      <c r="B1943" s="2" t="s">
+        <v>3273</v>
+      </c>
+      <c r="C1943" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1943" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1943" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1943" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1943" s="2" t="s">
+        <v>3277</v>
+      </c>
+      <c r="H1943" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1943" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1943" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1943" s="2" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1943" s="2" t="s">
+        <v>3275</v>
+      </c>
+    </row>
+    <row r="1944" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1944" s="2" t="s">
+        <v>3278</v>
+      </c>
+      <c r="B1944" s="2" t="s">
+        <v>3273</v>
+      </c>
+      <c r="C1944" s="1">
+        <v>45118</v>
+      </c>
+      <c r="D1944" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1944" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1944" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1944" s="2" t="s">
+        <v>3279</v>
+      </c>
+      <c r="H1944" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1944" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1944" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1944" s="2" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1944" s="2" t="s">
+        <v>3275</v>
+      </c>
+    </row>
+    <row r="1945" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1945" s="2" t="s">
+        <v>3280</v>
+      </c>
+      <c r="B1945" s="2" t="s">
+        <v>3281</v>
+      </c>
+      <c r="C1945" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1945" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1945" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1945" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1945" s="2" t="s">
+        <v>3283</v>
+      </c>
+      <c r="H1945" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1945" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1945" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1945" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1945" s="2" t="s">
+        <v>3284</v>
+      </c>
+      <c r="Q1945" t="s">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="1946" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1946" s="2" t="s">
+        <v>3286</v>
+      </c>
+      <c r="B1946" s="2" t="s">
+        <v>3281</v>
+      </c>
+      <c r="C1946" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1946" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1946" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1946" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1946" s="2" t="s">
+        <v>3287</v>
+      </c>
+      <c r="H1946" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1946" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1946" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1946" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1946" s="2" t="s">
+        <v>3284</v>
+      </c>
+      <c r="Q1946" t="s">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1947" s="2" t="s">
+        <v>3288</v>
+      </c>
+      <c r="B1947" s="2" t="s">
+        <v>3281</v>
+      </c>
+      <c r="C1947" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1947" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1947" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1947" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1947" s="2" t="s">
+        <v>3289</v>
+      </c>
+      <c r="H1947" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1947" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1947" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1947" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1947" s="2" t="s">
+        <v>3284</v>
+      </c>
+      <c r="Q1947" t="s">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="1948" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1948" s="2" t="s">
+        <v>3290</v>
+      </c>
+      <c r="B1948" s="2" t="s">
+        <v>3281</v>
+      </c>
+      <c r="C1948" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1948" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1948" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1948" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1948" s="2" t="s">
+        <v>3291</v>
+      </c>
+      <c r="H1948" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1948" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1948" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1948" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1948" s="2" t="s">
+        <v>3284</v>
+      </c>
+      <c r="Q1948" t="s">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="1949" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1949" s="2" t="s">
+        <v>3292</v>
+      </c>
+      <c r="B1949" s="2" t="s">
+        <v>3281</v>
+      </c>
+      <c r="C1949" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1949" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1949" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1949" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1949" s="2" t="s">
+        <v>3293</v>
+      </c>
+      <c r="H1949" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1949" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1949" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1949" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1949" s="2" t="s">
+        <v>3284</v>
+      </c>
+      <c r="Q1949" t="s">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="1950" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1950" s="2" t="s">
+        <v>3294</v>
+      </c>
+      <c r="B1950" s="2" t="s">
+        <v>3281</v>
+      </c>
+      <c r="C1950" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1950" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1950" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1950" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1950" s="2" t="s">
+        <v>3295</v>
+      </c>
+      <c r="H1950" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1950" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1950" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1950" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1950" s="2" t="s">
+        <v>3284</v>
+      </c>
+      <c r="Q1950" t="s">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="1951" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1951" s="2" t="s">
+        <v>3296</v>
+      </c>
+      <c r="B1951" s="2" t="s">
+        <v>3297</v>
+      </c>
+      <c r="C1951" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1951" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1951" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1951" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1951" s="2" t="s">
+        <v>3298</v>
+      </c>
+      <c r="H1951" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1951" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1951" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1951" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1951" s="2" t="s">
+        <v>3284</v>
+      </c>
+      <c r="Q1951" t="s">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="1952" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1952" s="2" t="s">
+        <v>3300</v>
+      </c>
+      <c r="B1952" s="2" t="s">
+        <v>3297</v>
+      </c>
+      <c r="C1952" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1952" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1952" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1952" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1952" s="2" t="s">
+        <v>3301</v>
+      </c>
+      <c r="H1952" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1952" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1952" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1952" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1952" s="2" t="s">
+        <v>3284</v>
+      </c>
+      <c r="Q1952" t="s">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="1953" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1953" s="2" t="s">
+        <v>3302</v>
+      </c>
+      <c r="B1953" s="2" t="s">
+        <v>3297</v>
+      </c>
+      <c r="C1953" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1953" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1953" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1953" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1953" s="2" t="s">
+        <v>3303</v>
+      </c>
+      <c r="H1953" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1953" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1953" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1953" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1953" s="2" t="s">
+        <v>3284</v>
+      </c>
+      <c r="Q1953" t="s">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="1954" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1954" s="2" t="s">
+        <v>3304</v>
+      </c>
+      <c r="B1954" s="2" t="s">
+        <v>3297</v>
+      </c>
+      <c r="C1954" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1954" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1954" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1954" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1954" s="2" t="s">
+        <v>3305</v>
+      </c>
+      <c r="H1954" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1954" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1954" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1954" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="P1954" s="2" t="s">
+        <v>3284</v>
+      </c>
+      <c r="Q1954" t="s">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="1955" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1955" s="2" t="s">
+        <v>3306</v>
+      </c>
+      <c r="B1955" s="2" t="s">
+        <v>3307</v>
+      </c>
+      <c r="C1955" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1955" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1955" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1955" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1955" s="2" t="s">
+        <v>3308</v>
+      </c>
+      <c r="H1955" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1955" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1955" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1955" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1955" s="2" t="s">
+        <v>3309</v>
+      </c>
+    </row>
+    <row r="1956" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1956" s="2" t="s">
+        <v>3310</v>
+      </c>
+      <c r="B1956" s="2" t="s">
+        <v>3307</v>
+      </c>
+      <c r="C1956" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1956" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1956" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1956" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1956" s="2" t="s">
+        <v>3311</v>
+      </c>
+      <c r="H1956" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1956" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1956" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1956" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1956" s="2" t="s">
+        <v>3309</v>
+      </c>
+    </row>
+    <row r="1957" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1957" s="2" t="s">
+        <v>3312</v>
+      </c>
+      <c r="B1957" s="2" t="s">
+        <v>3307</v>
+      </c>
+      <c r="C1957" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1957" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1957" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1957" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1957" s="2" t="s">
+        <v>3313</v>
+      </c>
+      <c r="H1957" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1957" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1957" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1957" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1957" s="2" t="s">
+        <v>3309</v>
+      </c>
+    </row>
+    <row r="1958" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1958" s="2" t="s">
+        <v>3314</v>
+      </c>
+      <c r="B1958" s="2" t="s">
+        <v>3307</v>
+      </c>
+      <c r="C1958" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1958" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1958" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1958" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1958" s="2" t="s">
+        <v>3315</v>
+      </c>
+      <c r="H1958" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1958" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1958" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1958" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1958" s="2" t="s">
+        <v>3309</v>
+      </c>
+    </row>
+    <row r="1959" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1959" s="2" t="s">
+        <v>3316</v>
+      </c>
+      <c r="B1959" s="2" t="s">
+        <v>3307</v>
+      </c>
+      <c r="C1959" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1959" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1959" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1959" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1959" s="2" t="s">
+        <v>3317</v>
+      </c>
+      <c r="H1959" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1959" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1959" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1959" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1959" s="2" t="s">
+        <v>3309</v>
+      </c>
+    </row>
+    <row r="1960" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1960" s="2" t="s">
+        <v>3318</v>
+      </c>
+      <c r="B1960" s="2" t="s">
+        <v>3319</v>
+      </c>
+      <c r="C1960" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1960" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1960" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1960" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1960" s="2" t="s">
+        <v>3320</v>
+      </c>
+      <c r="H1960" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1960" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1960" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1960" s="2" t="s">
+        <v>3136</v>
+      </c>
+      <c r="P1960" s="2" t="s">
+        <v>3321</v>
+      </c>
+      <c r="Q1960" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="1961" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1961" s="2" t="s">
+        <v>3322</v>
+      </c>
+      <c r="B1961" s="2" t="s">
+        <v>3319</v>
+      </c>
+      <c r="C1961" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1961" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1961" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1961" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1961" s="2" t="s">
+        <v>3323</v>
+      </c>
+      <c r="H1961" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1961" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1961" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1961" s="2" t="s">
+        <v>3136</v>
+      </c>
+      <c r="P1961" s="2" t="s">
+        <v>3321</v>
+      </c>
+      <c r="Q1961" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="1962" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1962" s="2" t="s">
+        <v>3324</v>
+      </c>
+      <c r="B1962" s="2" t="s">
+        <v>3325</v>
+      </c>
+      <c r="C1962" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1962" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1962" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1962" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1962" s="2" t="s">
+        <v>3326</v>
+      </c>
+      <c r="H1962" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1962" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1962" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1962" s="2" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1962" s="2" t="s">
+        <v>3327</v>
+      </c>
+      <c r="Q1962" t="s">
+        <v>3330</v>
+      </c>
+    </row>
+    <row r="1963" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1963" s="2" t="s">
+        <v>3328</v>
+      </c>
+      <c r="B1963" s="2" t="s">
+        <v>3325</v>
+      </c>
+      <c r="C1963" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1963" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1963" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1963" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1963" s="2" t="s">
+        <v>3329</v>
+      </c>
+      <c r="H1963" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1963" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1963" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1963" s="2" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1963" s="2" t="s">
+        <v>3327</v>
+      </c>
+      <c r="Q1963" t="s">
+        <v>3330</v>
+      </c>
+    </row>
+    <row r="1964" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1964" s="2" t="s">
+        <v>3333</v>
+      </c>
+      <c r="B1964" s="2" t="s">
+        <v>3325</v>
+      </c>
+      <c r="C1964" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1964" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1964" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1964" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1964" s="2" t="s">
+        <v>3332</v>
+      </c>
+      <c r="H1964" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1964" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1964" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1964" s="2" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1964" s="2" t="s">
+        <v>3327</v>
+      </c>
+      <c r="Q1964" t="s">
+        <v>3331</v>
+      </c>
+    </row>
+    <row r="1965" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1965" s="2" t="s">
+        <v>3334</v>
+      </c>
+      <c r="B1965" s="2" t="s">
+        <v>3325</v>
+      </c>
+      <c r="C1965" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1965" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1965" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1965" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1965" s="2" t="s">
+        <v>3335</v>
+      </c>
+      <c r="H1965" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1965" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1965" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1965" s="2" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1965" s="2" t="s">
+        <v>3327</v>
+      </c>
+      <c r="Q1965" t="s">
+        <v>3331</v>
+      </c>
+    </row>
+    <row r="1966" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1966" s="2" t="s">
+        <v>3336</v>
+      </c>
+      <c r="B1966" s="2" t="s">
+        <v>3325</v>
+      </c>
+      <c r="C1966" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1966" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1966" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1966" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1966" s="2" t="s">
+        <v>3337</v>
+      </c>
+      <c r="H1966" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1966" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1966" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1966" s="2" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1966" s="2" t="s">
+        <v>3327</v>
+      </c>
+      <c r="Q1966" t="s">
+        <v>3338</v>
+      </c>
+    </row>
+    <row r="1967" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1967" s="2" t="s">
+        <v>3339</v>
+      </c>
+      <c r="B1967" s="2" t="s">
+        <v>3325</v>
+      </c>
+      <c r="C1967" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1967" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1967" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1967" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1967" s="2" t="s">
+        <v>3340</v>
+      </c>
+      <c r="H1967" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1967" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1967" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1967" s="2" t="s">
+        <v>3127</v>
+      </c>
+      <c r="P1967" s="2" t="s">
+        <v>3327</v>
+      </c>
+      <c r="Q1967" t="s">
+        <v>3341</v>
+      </c>
+    </row>
+    <row r="1968" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1968" s="2" t="s">
+        <v>3342</v>
+      </c>
+      <c r="B1968" s="2" t="s">
+        <v>3343</v>
+      </c>
+      <c r="C1968" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1968" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1968" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1968" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1968" s="2" t="s">
+        <v>3344</v>
+      </c>
+      <c r="H1968" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1968" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1968" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1968" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1968" s="2" t="s">
+        <v>3345</v>
+      </c>
+      <c r="Q1968" t="s">
+        <v>3346</v>
+      </c>
+    </row>
+    <row r="1969" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1969" s="2" t="s">
+        <v>3347</v>
+      </c>
+      <c r="B1969" s="2" t="s">
+        <v>3343</v>
+      </c>
+      <c r="C1969" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="D1969" s="2" t="s">
+        <v>3125</v>
+      </c>
+      <c r="E1969" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1969" s="2">
+        <v>30</v>
+      </c>
+      <c r="G1969" s="2" t="s">
+        <v>3348</v>
+      </c>
+      <c r="H1969" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1969" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1969" s="2" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O1969" s="2" t="s">
+        <v>3145</v>
+      </c>
+      <c r="P1969" s="2" t="s">
+        <v>3345</v>
+      </c>
+      <c r="Q1969" t="s">
+        <v>3346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>